<commit_message>
cambios CU registrar solicitud
</commit_message>
<xml_diff>
--- a/NUEVO Matriz de actividades.xlsx
+++ b/NUEVO Matriz de actividades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t xml:space="preserve">Matriz de actividades vs Casos de Uso </t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t xml:space="preserve">El sistema debe verificar si los archivos subidos </t>
+  </si>
+  <si>
+    <t>El sistema envia un correo al solicitante con el código de solicitud, el cual permite ver el estado de la solicitud</t>
+  </si>
+  <si>
+    <t>RF15</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -493,13 +499,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -543,11 +545,108 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -560,105 +659,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -947,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:K36"/>
+  <dimension ref="D3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J7"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,490 +982,507 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="40"/>
     </row>
     <row r="4" spans="4:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="50"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="54" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="60" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="52" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="4:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="57"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="63"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="53"/>
     </row>
     <row r="6" spans="4:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="26" t="s">
+      <c r="I6" s="56"/>
+      <c r="J6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="63" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="4:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="25"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="6" t="s">
+    <row r="7" spans="4:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="34"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="56"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="64"/>
+    </row>
+    <row r="8" spans="4:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="34"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="25"/>
-      <c r="E8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="45"/>
-      <c r="J8" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="H8" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="57"/>
       <c r="K8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="4:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="25"/>
-      <c r="E9" s="3" t="s">
+    <row r="9" spans="4:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="34"/>
+      <c r="E9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="62"/>
+      <c r="J9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="34"/>
+      <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="24" t="s">
+      <c r="G10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="6" t="s">
+      <c r="I10" s="56"/>
+      <c r="J10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="4:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="25"/>
-      <c r="E10" s="27" t="s">
+    <row r="11" spans="4:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="34"/>
+      <c r="E11" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F11" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="24" t="s">
+      <c r="G11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="28" t="s">
+      <c r="I11" s="56"/>
+      <c r="J11" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K11" s="56" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="4:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="25"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="24" t="s">
+    <row r="12" spans="4:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="34"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="24"/>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="56"/>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D13" s="19"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="19"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="19"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="22"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="19"/>
-      <c r="E16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="16"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="19"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="19"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="40"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="16"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="16"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="26" spans="4:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="46" t="s">
+      <c r="D19" s="17"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="27" spans="4:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="48"/>
-    </row>
-    <row r="27" spans="4:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D27" s="49" t="s">
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="40"/>
+    </row>
+    <row r="28" spans="4:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D28" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="54" t="s">
+      <c r="E28" s="42"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="55"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="60" t="s">
+      <c r="H28" s="45"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="62" t="s">
+      <c r="K28" s="52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="4:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D28" s="52" t="s">
+    <row r="29" spans="4:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E29" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="53" t="s">
+      <c r="F29" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="57"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="63"/>
-    </row>
-    <row r="29" spans="4:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="25" t="s">
+      <c r="G29" s="47"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="4:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E30" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="36" t="s">
+      <c r="G30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="37"/>
-      <c r="J29" s="34" t="s">
+      <c r="I30" s="28"/>
+      <c r="J30" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="K29" s="32" t="s">
+      <c r="K30" s="29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="4:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="25"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="24" t="s">
+    <row r="31" spans="4:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="34"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="42"/>
-    </row>
-    <row r="31" spans="4:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="25"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H31" s="36" t="s">
+      <c r="I31" s="56"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="30"/>
+    </row>
+    <row r="32" spans="4:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="34"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="I31" s="37"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="33"/>
-    </row>
-    <row r="32" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D32" s="25"/>
-      <c r="E32" s="14" t="s">
+      <c r="I32" s="28"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="4:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="D33" s="34"/>
+      <c r="E33" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F33" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="36" t="s">
+      <c r="G33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="37"/>
-      <c r="J32" s="6" t="s">
+      <c r="I33" s="28"/>
+      <c r="J33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="K33" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D33" s="25"/>
-      <c r="E33" s="14" t="s">
+    <row r="34" spans="4:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="D34" s="34"/>
+      <c r="E34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F34" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H33" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="I33" s="37"/>
-      <c r="J33" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="4:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="D34" s="25"/>
-      <c r="E34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H34" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="37"/>
-      <c r="J34" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="25"/>
-      <c r="E35" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="F35" s="38" t="s">
-        <v>23</v>
+      <c r="H34" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="I34" s="28"/>
+      <c r="J34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="D35" s="34"/>
+      <c r="E35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H35" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35" s="37"/>
-      <c r="J35" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="12" t="s">
+      <c r="H35" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I35" s="28"/>
+      <c r="J35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="4:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="25"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="39"/>
+    <row r="36" spans="4:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="34"/>
+      <c r="E36" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>23</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="36" t="s">
+      <c r="H36" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="28"/>
+      <c r="J36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="34"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="55"/>
+      <c r="G37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="I36" s="37"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="12" t="s">
+      <c r="I37" s="28"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="10" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="D29:D36"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="F29:F31"/>
+  <mergeCells count="42">
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="D6:D12"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="D3:K3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="G4:I5"/>
+    <mergeCell ref="D30:D37"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="H31:I31"/>
     <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K30:K32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="E36:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>